<commit_message>
Fixed a question in the queries file
</commit_message>
<xml_diff>
--- a/queries.xlsx
+++ b/queries.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NlpExercises\Ex3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\NlpExercises\nlp-ex3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94D02DEA-86C4-4EEF-B4F3-D4C132C7BB6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{508C4247-6F04-43D7-946B-2C762B9E4CD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="12432" xr2:uid="{8B97D1D5-E4BC-4844-BA03-A5908995EEA0}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{8B97D1D5-E4BC-4844-BA03-A5908995EEA0}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="87">
   <si>
     <t>Page Id</t>
   </si>
@@ -348,6 +348,9 @@
   </si>
   <si>
     <t>האם משרתי חובה יכולים להצביע לבחירות הארציות בקלפי אזרחי?</t>
+  </si>
+  <si>
+    <t>באיזה שפות יש קורס פסיכומטרי ללא עלות?</t>
   </si>
 </sst>
 </file>
@@ -705,8 +708,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F4A92707-B455-4818-8F3F-73DAD111D05A}">
   <dimension ref="A1:E21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="B13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -784,7 +787,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>19</v>
       </c>
@@ -801,7 +804,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>24</v>
       </c>
@@ -818,7 +821,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="172.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="144" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>27</v>
       </c>
@@ -852,7 +855,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="100.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>36</v>
       </c>
@@ -943,6 +946,9 @@
       </c>
       <c r="B14" s="1" t="s">
         <v>57</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>86</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>10</v>

</xml_diff>